<commit_message>
Updated PDF Merger to latest version
</commit_message>
<xml_diff>
--- a/charts_xlsx/jcchart.xlsx
+++ b/charts_xlsx/jcchart.xlsx
@@ -40,16 +40,16 @@
     <t>Asc</t>
   </si>
   <si>
-    <t>Sun Aspect Score</t>
-  </si>
-  <si>
-    <t>Moon Aspect Score</t>
-  </si>
-  <si>
-    <t>Asc Aspect Score</t>
-  </si>
-  <si>
-    <t>Personal total</t>
+    <t>Sun Aspect Intensity</t>
+  </si>
+  <si>
+    <t>Moon Aspect Intensity</t>
+  </si>
+  <si>
+    <t>Asc Aspect Intensity</t>
+  </si>
+  <si>
+    <t>Aspect intensity total</t>
   </si>
   <si>
     <t>Pattern</t>
@@ -1307,6 +1307,10 @@
       <c r="L2">
         <v>7</v>
       </c>
+      <c r="M2">
+        <f>SUM(J1:L1)</f>
+        <v>0</v>
+      </c>
       <c r="Q2">
         <v>1</v>
       </c>
@@ -1339,6 +1343,10 @@
       <c r="K3">
         <v>10</v>
       </c>
+      <c r="M3">
+        <f>SUM(J2:L2)</f>
+        <v>0</v>
+      </c>
       <c r="P3" t="s">
         <v>69</v>
       </c>
@@ -1380,6 +1388,10 @@
       <c r="L4">
         <v>2</v>
       </c>
+      <c r="M4">
+        <f>SUM(J3:L3)</f>
+        <v>0</v>
+      </c>
       <c r="P4" t="s">
         <v>74</v>
       </c>
@@ -1406,6 +1418,10 @@
       <c r="K5">
         <v>10</v>
       </c>
+      <c r="M5">
+        <f>SUM(J4:L4)</f>
+        <v>0</v>
+      </c>
       <c r="Q5">
         <v>4</v>
       </c>
@@ -1429,6 +1445,10 @@
       <c r="K6">
         <v>10</v>
       </c>
+      <c r="M6">
+        <f>SUM(J5:L5)</f>
+        <v>0</v>
+      </c>
       <c r="Q6">
         <v>5</v>
       </c>
@@ -1446,6 +1466,10 @@
       <c r="L7">
         <v>6</v>
       </c>
+      <c r="M7">
+        <f>SUM(J6:L6)</f>
+        <v>0</v>
+      </c>
       <c r="Q7">
         <v>6</v>
       </c>
@@ -1463,6 +1487,10 @@
       <c r="L8">
         <v>6</v>
       </c>
+      <c r="M8">
+        <f>SUM(J7:L7)</f>
+        <v>0</v>
+      </c>
       <c r="Q8">
         <v>7</v>
       </c>
@@ -1480,6 +1508,10 @@
       <c r="L9">
         <v>6</v>
       </c>
+      <c r="M9">
+        <f>SUM(J8:L8)</f>
+        <v>0</v>
+      </c>
       <c r="Q9">
         <v>8</v>
       </c>
@@ -1503,6 +1535,10 @@
       <c r="L10">
         <v>6</v>
       </c>
+      <c r="M10">
+        <f>SUM(J9:L9)</f>
+        <v>0</v>
+      </c>
       <c r="Q10">
         <v>9</v>
       </c>
@@ -1526,6 +1562,10 @@
       <c r="K11">
         <v>5</v>
       </c>
+      <c r="M11">
+        <f>SUM(J10:L10)</f>
+        <v>0</v>
+      </c>
       <c r="Q11">
         <v>10</v>
       </c>
@@ -1543,6 +1583,10 @@
       <c r="K12">
         <v>5</v>
       </c>
+      <c r="M12">
+        <f>SUM(J11:L11)</f>
+        <v>0</v>
+      </c>
       <c r="Q12">
         <v>11</v>
       </c>
@@ -1554,6 +1598,10 @@
       <c r="F13" t="s">
         <v>89</v>
       </c>
+      <c r="M13">
+        <f>SUM(J12:L12)</f>
+        <v>0</v>
+      </c>
       <c r="Q13">
         <v>12</v>
       </c>
@@ -1577,6 +1625,10 @@
       <c r="L14">
         <v>8</v>
       </c>
+      <c r="M14">
+        <f>SUM(J13:L13)</f>
+        <v>0</v>
+      </c>
       <c r="Q14">
         <v>13</v>
       </c>
@@ -1606,6 +1658,10 @@
       <c r="L15">
         <v>8</v>
       </c>
+      <c r="M15">
+        <f>SUM(J14:L14)</f>
+        <v>0</v>
+      </c>
       <c r="Q15">
         <v>14</v>
       </c>
@@ -1623,6 +1679,10 @@
       <c r="L16">
         <v>8</v>
       </c>
+      <c r="M16">
+        <f>SUM(J15:L15)</f>
+        <v>0</v>
+      </c>
       <c r="Q16">
         <v>15</v>
       </c>
@@ -1652,6 +1712,10 @@
       <c r="L17">
         <v>8</v>
       </c>
+      <c r="M17">
+        <f>SUM(J16:L16)</f>
+        <v>0</v>
+      </c>
       <c r="Q17">
         <v>16</v>
       </c>
@@ -1681,6 +1745,10 @@
       <c r="L18">
         <v>8</v>
       </c>
+      <c r="M18">
+        <f>SUM(J17:L17)</f>
+        <v>0</v>
+      </c>
       <c r="Q18">
         <v>17</v>
       </c>
@@ -1704,6 +1772,10 @@
       <c r="K19">
         <v>7</v>
       </c>
+      <c r="M19">
+        <f>SUM(J18:L18)</f>
+        <v>0</v>
+      </c>
       <c r="Q19">
         <v>18</v>
       </c>
@@ -1727,6 +1799,10 @@
       <c r="K20">
         <v>7</v>
       </c>
+      <c r="M20">
+        <f>SUM(J19:L19)</f>
+        <v>0</v>
+      </c>
       <c r="Q20">
         <v>19</v>
       </c>
@@ -1744,6 +1820,10 @@
       <c r="J21">
         <v>2</v>
       </c>
+      <c r="M21">
+        <f>SUM(J20:L20)</f>
+        <v>0</v>
+      </c>
       <c r="Q21">
         <v>20</v>
       </c>
@@ -1767,6 +1847,10 @@
       <c r="L22">
         <v>1.5</v>
       </c>
+      <c r="M22">
+        <f>SUM(J21:L21)</f>
+        <v>0</v>
+      </c>
       <c r="Q22">
         <v>21</v>
       </c>
@@ -1784,6 +1868,10 @@
       <c r="L23">
         <v>4</v>
       </c>
+      <c r="M23">
+        <f>SUM(J22:L22)</f>
+        <v>0</v>
+      </c>
       <c r="Q23">
         <v>22</v>
       </c>
@@ -1813,6 +1901,10 @@
       <c r="L24">
         <v>4</v>
       </c>
+      <c r="M24">
+        <f>SUM(J23:L23)</f>
+        <v>0</v>
+      </c>
       <c r="Q24">
         <v>23</v>
       </c>
@@ -1836,6 +1928,10 @@
       <c r="K25">
         <v>6</v>
       </c>
+      <c r="M25">
+        <f>SUM(J24:L24)</f>
+        <v>0</v>
+      </c>
       <c r="Q25">
         <v>24</v>
       </c>
@@ -1859,6 +1955,10 @@
       <c r="K26">
         <v>6</v>
       </c>
+      <c r="M26">
+        <f>SUM(J25:L25)</f>
+        <v>0</v>
+      </c>
       <c r="Q26">
         <v>25</v>
       </c>
@@ -1882,6 +1982,10 @@
       <c r="K27">
         <v>6</v>
       </c>
+      <c r="M27">
+        <f>SUM(J26:L26)</f>
+        <v>0</v>
+      </c>
       <c r="Q27">
         <v>26</v>
       </c>
@@ -1905,6 +2009,10 @@
       <c r="K28">
         <v>6</v>
       </c>
+      <c r="M28">
+        <f>SUM(J27:L27)</f>
+        <v>0</v>
+      </c>
       <c r="Q28">
         <v>27</v>
       </c>
@@ -1922,6 +2030,10 @@
       <c r="L29">
         <v>9</v>
       </c>
+      <c r="M29">
+        <f>SUM(J28:L28)</f>
+        <v>0</v>
+      </c>
       <c r="Q29">
         <v>28</v>
       </c>
@@ -1939,6 +2051,10 @@
       <c r="L30">
         <v>9</v>
       </c>
+      <c r="M30">
+        <f>SUM(J29:L29)</f>
+        <v>0</v>
+      </c>
       <c r="Q30">
         <v>29</v>
       </c>
@@ -1968,6 +2084,10 @@
       <c r="L31">
         <v>9</v>
       </c>
+      <c r="M31">
+        <f>SUM(J30:L30)</f>
+        <v>0</v>
+      </c>
       <c r="Q31">
         <v>30</v>
       </c>
@@ -1997,6 +2117,10 @@
       <c r="L32">
         <v>9</v>
       </c>
+      <c r="M32">
+        <f>SUM(J31:L31)</f>
+        <v>0</v>
+      </c>
       <c r="Q32">
         <v>31</v>
       </c>
@@ -2026,6 +2150,10 @@
       <c r="L33">
         <v>9</v>
       </c>
+      <c r="M33">
+        <f>SUM(J32:L32)</f>
+        <v>0</v>
+      </c>
       <c r="Q33">
         <v>32</v>
       </c>
@@ -2049,6 +2177,10 @@
       <c r="K34">
         <v>8</v>
       </c>
+      <c r="M34">
+        <f>SUM(J33:L33)</f>
+        <v>0</v>
+      </c>
       <c r="Q34">
         <v>33</v>
       </c>
@@ -2072,6 +2204,10 @@
       <c r="K35">
         <v>8</v>
       </c>
+      <c r="M35">
+        <f>SUM(J34:L34)</f>
+        <v>0</v>
+      </c>
       <c r="Q35">
         <v>34</v>
       </c>
@@ -2089,6 +2225,10 @@
       <c r="K36">
         <v>8</v>
       </c>
+      <c r="M36">
+        <f>SUM(J35:L35)</f>
+        <v>0</v>
+      </c>
       <c r="Q36">
         <v>35</v>
       </c>
@@ -2100,6 +2240,10 @@
       <c r="F37" t="s">
         <v>139</v>
       </c>
+      <c r="M37">
+        <f>SUM(J36:L36)</f>
+        <v>0</v>
+      </c>
       <c r="Q37">
         <v>36</v>
       </c>
@@ -2117,6 +2261,10 @@
       <c r="L38">
         <v>4</v>
       </c>
+      <c r="M38">
+        <f>SUM(J37:L37)</f>
+        <v>0</v>
+      </c>
       <c r="Q38">
         <v>37</v>
       </c>
@@ -2140,6 +2288,10 @@
       <c r="L39">
         <v>4</v>
       </c>
+      <c r="M39">
+        <f>SUM(J38:L38)</f>
+        <v>0</v>
+      </c>
       <c r="Q39">
         <v>38</v>
       </c>
@@ -2163,6 +2315,10 @@
       <c r="K40">
         <v>1.5</v>
       </c>
+      <c r="M40">
+        <f>SUM(J39:L39)</f>
+        <v>0</v>
+      </c>
       <c r="Q40">
         <v>39</v>
       </c>
@@ -2192,6 +2348,10 @@
       <c r="K41">
         <v>4</v>
       </c>
+      <c r="M41">
+        <f>SUM(J40:L40)</f>
+        <v>0</v>
+      </c>
       <c r="Q41">
         <v>40</v>
       </c>
@@ -2209,6 +2369,10 @@
       <c r="K42">
         <v>4</v>
       </c>
+      <c r="M42">
+        <f>SUM(J41:L41)</f>
+        <v>0</v>
+      </c>
       <c r="Q42">
         <v>41</v>
       </c>
@@ -2220,6 +2384,10 @@
       <c r="F43" t="s">
         <v>153</v>
       </c>
+      <c r="M43">
+        <f>SUM(J42:L42)</f>
+        <v>0</v>
+      </c>
       <c r="Q43">
         <v>42</v>
       </c>
@@ -2237,6 +2405,10 @@
       <c r="L44">
         <v>8</v>
       </c>
+      <c r="M44">
+        <f>SUM(J43:L43)</f>
+        <v>0</v>
+      </c>
       <c r="Q44">
         <v>43</v>
       </c>
@@ -2254,6 +2426,10 @@
       <c r="L45">
         <v>8</v>
       </c>
+      <c r="M45">
+        <f>SUM(J44:L44)</f>
+        <v>0</v>
+      </c>
       <c r="Q45">
         <v>44</v>
       </c>
@@ -2283,6 +2459,10 @@
       <c r="L46">
         <v>8</v>
       </c>
+      <c r="M46">
+        <f>SUM(J45:L45)</f>
+        <v>0</v>
+      </c>
       <c r="Q46">
         <v>45</v>
       </c>
@@ -2312,6 +2492,10 @@
       <c r="L47">
         <v>8</v>
       </c>
+      <c r="M47">
+        <f>SUM(J46:L46)</f>
+        <v>0</v>
+      </c>
       <c r="Q47">
         <v>46</v>
       </c>
@@ -2341,6 +2525,10 @@
       <c r="L48">
         <v>8</v>
       </c>
+      <c r="M48">
+        <f>SUM(J47:L47)</f>
+        <v>0</v>
+      </c>
       <c r="Q48">
         <v>47</v>
       </c>
@@ -2364,6 +2552,10 @@
       <c r="K49">
         <v>9</v>
       </c>
+      <c r="M49">
+        <f>SUM(J48:L48)</f>
+        <v>0</v>
+      </c>
       <c r="Q49">
         <v>48</v>
       </c>
@@ -2387,6 +2579,10 @@
       <c r="K50">
         <v>9</v>
       </c>
+      <c r="M50">
+        <f>SUM(J49:L49)</f>
+        <v>0</v>
+      </c>
       <c r="Q50">
         <v>49</v>
       </c>
@@ -2416,6 +2612,10 @@
       <c r="K51">
         <v>9</v>
       </c>
+      <c r="M51">
+        <f>SUM(J50:L50)</f>
+        <v>0</v>
+      </c>
       <c r="Q51">
         <v>50</v>
       </c>
@@ -2433,6 +2633,10 @@
       <c r="L52">
         <v>6</v>
       </c>
+      <c r="M52">
+        <f>SUM(J51:L51)</f>
+        <v>0</v>
+      </c>
       <c r="Q52">
         <v>51</v>
       </c>
@@ -2450,6 +2654,10 @@
       <c r="L53">
         <v>6</v>
       </c>
+      <c r="M53">
+        <f>SUM(J52:L52)</f>
+        <v>0</v>
+      </c>
       <c r="Q53">
         <v>52</v>
       </c>
@@ -2467,6 +2675,10 @@
       <c r="L54">
         <v>6</v>
       </c>
+      <c r="M54">
+        <f>SUM(J53:L53)</f>
+        <v>0</v>
+      </c>
       <c r="Q54">
         <v>53</v>
       </c>
@@ -2490,6 +2702,10 @@
       <c r="L55">
         <v>6</v>
       </c>
+      <c r="M55">
+        <f>SUM(J54:L54)</f>
+        <v>0</v>
+      </c>
       <c r="Q55">
         <v>54</v>
       </c>
@@ -2513,6 +2729,10 @@
       <c r="K56">
         <v>4</v>
       </c>
+      <c r="M56">
+        <f>SUM(J55:L55)</f>
+        <v>0</v>
+      </c>
       <c r="Q56">
         <v>55</v>
       </c>
@@ -2530,6 +2750,10 @@
       <c r="K57">
         <v>4</v>
       </c>
+      <c r="M57">
+        <f>SUM(J56:L56)</f>
+        <v>0</v>
+      </c>
       <c r="Q57">
         <v>56</v>
       </c>
@@ -2541,6 +2765,10 @@
       <c r="F58" t="s">
         <v>185</v>
       </c>
+      <c r="M58">
+        <f>SUM(J57:L57)</f>
+        <v>0</v>
+      </c>
       <c r="Q58">
         <v>57</v>
       </c>
@@ -2558,6 +2786,10 @@
       <c r="F59" t="s">
         <v>187</v>
       </c>
+      <c r="M59">
+        <f>SUM(J58:L58)</f>
+        <v>0</v>
+      </c>
       <c r="Q59">
         <v>58</v>
       </c>
@@ -2575,6 +2807,10 @@
       <c r="L60">
         <v>7</v>
       </c>
+      <c r="M60">
+        <f>SUM(J59:L59)</f>
+        <v>0</v>
+      </c>
       <c r="Q60">
         <v>59</v>
       </c>
@@ -2598,6 +2834,10 @@
       <c r="L61">
         <v>7</v>
       </c>
+      <c r="M61">
+        <f>SUM(J60:L60)</f>
+        <v>0</v>
+      </c>
       <c r="Q61">
         <v>60</v>
       </c>
@@ -2627,6 +2867,10 @@
       <c r="L62">
         <v>7</v>
       </c>
+      <c r="M62">
+        <f>SUM(J61:L61)</f>
+        <v>0</v>
+      </c>
       <c r="Q62">
         <v>61</v>
       </c>
@@ -2650,6 +2894,10 @@
       <c r="K63">
         <v>8</v>
       </c>
+      <c r="M63">
+        <f>SUM(J62:L62)</f>
+        <v>0</v>
+      </c>
       <c r="Q63">
         <v>62</v>
       </c>
@@ -2673,6 +2921,10 @@
       <c r="K64">
         <v>8</v>
       </c>
+      <c r="M64">
+        <f>SUM(J63:L63)</f>
+        <v>0</v>
+      </c>
       <c r="Q64">
         <v>63</v>
       </c>
@@ -2696,6 +2948,10 @@
       <c r="K65">
         <v>8</v>
       </c>
+      <c r="M65">
+        <f>SUM(J64:L64)</f>
+        <v>0</v>
+      </c>
       <c r="Q65">
         <v>64</v>
       </c>
@@ -2713,6 +2969,10 @@
       <c r="K66">
         <v>8</v>
       </c>
+      <c r="M66">
+        <f>SUM(J65:L65)</f>
+        <v>0</v>
+      </c>
       <c r="Q66">
         <v>65</v>
       </c>
@@ -2730,6 +2990,10 @@
       <c r="F67" t="s">
         <v>205</v>
       </c>
+      <c r="M67">
+        <f>SUM(J66:L66)</f>
+        <v>0</v>
+      </c>
       <c r="Q67">
         <v>66</v>
       </c>
@@ -2747,6 +3011,10 @@
       <c r="L68">
         <v>5</v>
       </c>
+      <c r="M68">
+        <f>SUM(J67:L67)</f>
+        <v>0</v>
+      </c>
       <c r="Q68">
         <v>67</v>
       </c>
@@ -2776,6 +3044,10 @@
       <c r="L69">
         <v>5</v>
       </c>
+      <c r="M69">
+        <f>SUM(J68:L68)</f>
+        <v>0</v>
+      </c>
       <c r="Q69">
         <v>68</v>
       </c>
@@ -2799,6 +3071,10 @@
       <c r="K70">
         <v>6</v>
       </c>
+      <c r="M70">
+        <f>SUM(J69:L69)</f>
+        <v>0</v>
+      </c>
       <c r="Q70">
         <v>69</v>
       </c>
@@ -2822,6 +3098,10 @@
       <c r="K71">
         <v>6</v>
       </c>
+      <c r="M71">
+        <f>SUM(J70:L70)</f>
+        <v>0</v>
+      </c>
       <c r="Q71">
         <v>70</v>
       </c>
@@ -2845,6 +3125,10 @@
       <c r="K72">
         <v>6</v>
       </c>
+      <c r="M72">
+        <f>SUM(J71:L71)</f>
+        <v>0</v>
+      </c>
       <c r="Q72">
         <v>71</v>
       </c>
@@ -2868,6 +3152,10 @@
       <c r="K73">
         <v>6</v>
       </c>
+      <c r="M73">
+        <f>SUM(J72:L72)</f>
+        <v>0</v>
+      </c>
       <c r="Q73">
         <v>72</v>
       </c>
@@ -2885,6 +3173,10 @@
       <c r="L74">
         <v>10</v>
       </c>
+      <c r="M74">
+        <f>SUM(J73:L73)</f>
+        <v>0</v>
+      </c>
       <c r="Q74">
         <v>73</v>
       </c>
@@ -2902,6 +3194,10 @@
       <c r="L75">
         <v>10</v>
       </c>
+      <c r="M75">
+        <f>SUM(J74:L74)</f>
+        <v>0</v>
+      </c>
       <c r="Q75">
         <v>74</v>
       </c>
@@ -2925,6 +3221,10 @@
       <c r="L76">
         <v>10</v>
       </c>
+      <c r="M76">
+        <f>SUM(J75:L75)</f>
+        <v>0</v>
+      </c>
       <c r="Q76">
         <v>75</v>
       </c>
@@ -2954,6 +3254,10 @@
       <c r="L77">
         <v>10</v>
       </c>
+      <c r="M77">
+        <f>SUM(J76:L76)</f>
+        <v>0</v>
+      </c>
       <c r="Q77">
         <v>76</v>
       </c>
@@ -2983,6 +3287,10 @@
       <c r="L78">
         <v>10</v>
       </c>
+      <c r="M78">
+        <f>SUM(J77:L77)</f>
+        <v>0</v>
+      </c>
       <c r="Q78">
         <v>77</v>
       </c>
@@ -3006,6 +3314,10 @@
       <c r="K79">
         <v>7</v>
       </c>
+      <c r="M79">
+        <f>SUM(J78:L78)</f>
+        <v>0</v>
+      </c>
       <c r="Q79">
         <v>78</v>
       </c>
@@ -3029,6 +3341,10 @@
       <c r="K80">
         <v>7</v>
       </c>
+      <c r="M80">
+        <f>SUM(J79:L79)</f>
+        <v>0</v>
+      </c>
       <c r="Q80">
         <v>79</v>
       </c>
@@ -3040,6 +3356,10 @@
       <c r="F81" t="s">
         <v>237</v>
       </c>
+      <c r="M81">
+        <f>SUM(J80:L80)</f>
+        <v>0</v>
+      </c>
       <c r="Q81">
         <v>80</v>
       </c>
@@ -3051,6 +3371,10 @@
       <c r="F82" t="s">
         <v>239</v>
       </c>
+      <c r="M82">
+        <f>SUM(J81:L81)</f>
+        <v>0</v>
+      </c>
       <c r="Q82">
         <v>81</v>
       </c>
@@ -3068,6 +3392,10 @@
       <c r="L83">
         <v>5</v>
       </c>
+      <c r="M83">
+        <f>SUM(J82:L82)</f>
+        <v>0</v>
+      </c>
       <c r="Q83">
         <v>82</v>
       </c>
@@ -3091,6 +3419,10 @@
       <c r="L84">
         <v>5</v>
       </c>
+      <c r="M84">
+        <f>SUM(J83:L83)</f>
+        <v>0</v>
+      </c>
       <c r="Q84">
         <v>83</v>
       </c>
@@ -3108,6 +3440,10 @@
       <c r="J85">
         <v>5</v>
       </c>
+      <c r="M85">
+        <f>SUM(J84:L84)</f>
+        <v>0</v>
+      </c>
       <c r="Q85">
         <v>84</v>
       </c>
@@ -3131,6 +3467,10 @@
       <c r="K86">
         <v>5</v>
       </c>
+      <c r="M86">
+        <f>SUM(J85:L85)</f>
+        <v>0</v>
+      </c>
       <c r="Q86">
         <v>85</v>
       </c>
@@ -3154,6 +3494,10 @@
       <c r="L87">
         <v>3</v>
       </c>
+      <c r="M87">
+        <f>SUM(J86:L86)</f>
+        <v>0</v>
+      </c>
       <c r="Q87">
         <v>86</v>
       </c>
@@ -3171,6 +3515,10 @@
       <c r="L88">
         <v>3</v>
       </c>
+      <c r="M88">
+        <f>SUM(J87:L87)</f>
+        <v>0</v>
+      </c>
       <c r="Q88">
         <v>87</v>
       </c>
@@ -3182,6 +3530,10 @@
       <c r="F89" t="s">
         <v>255</v>
       </c>
+      <c r="M89">
+        <f>SUM(J88:L88)</f>
+        <v>0</v>
+      </c>
       <c r="Q89">
         <v>88</v>
       </c>
@@ -3205,6 +3557,10 @@
       <c r="L90">
         <v>7</v>
       </c>
+      <c r="M90">
+        <f>SUM(J89:L89)</f>
+        <v>0</v>
+      </c>
       <c r="Q90">
         <v>89</v>
       </c>
@@ -3233,6 +3589,10 @@
       </c>
       <c r="L91">
         <v>7</v>
+      </c>
+      <c r="M91">
+        <f>SUM(J90:L90)</f>
+        <v>0</v>
       </c>
       <c r="Q91">
         <v>90</v>

</xml_diff>